<commit_message>
IH 25APR2022 fix header for Supplementary Table 4.
</commit_message>
<xml_diff>
--- a/supplementary_tables/Supplementary_Tables.xlsx
+++ b/supplementary_tables/Supplementary_Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ianhoskins/satmut_utils_supplementary/supplementary_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{020C229C-98F2-5242-BD7C-D3665238CA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13340F8D-4E7F-1C40-8864-264F71B1DD17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="780" windowWidth="31440" windowHeight="19340" xr2:uid="{1B22F140-15A2-E942-BFF5-E35174637834}"/>
+    <workbookView xWindow="2620" yWindow="780" windowWidth="31440" windowHeight="19340" activeTab="3" xr2:uid="{1B22F140-15A2-E942-BFF5-E35174637834}"/>
   </bookViews>
   <sheets>
     <sheet name="Supplementary_Table_1" sheetId="1" r:id="rId1"/>
@@ -1707,20 +1707,20 @@
     <t>Supplementary Table 3: CBS tail-less primers for RACE-like, Anchored Multiplex PCR chemistry</t>
   </si>
   <si>
-    <t>Supplementary Table 3: CBS primers for negative control library amplification</t>
-  </si>
-  <si>
     <t>Supplementary Table 2: pDEST_HC_Rec_Bxb_v2_CBS PCR1 and PCR2 primers for amplicon chemistry</t>
   </si>
   <si>
     <t>Supplementary Table 1: Variants with differntial RNA abundance by amplicon and RACE-like chemistries</t>
+  </si>
+  <si>
+    <t>Supplementary Table 4: CBS primers for negative control library amplification</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1732,12 +1732,6 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Helvetica Neue"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -1773,7 +1767,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -2137,7 +2131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CDD16E8-C7C2-B243-8EF3-648BE6A0AF40}">
   <dimension ref="A1:T113"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" workbookViewId="0"/>
+    <sheetView zoomScale="68" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2155,7 +2149,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -9259,7 +9253,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -9870,8 +9864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17773C0-4ECC-EB44-AC66-28028E35A7C1}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9882,7 +9876,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
IH 26APR2022 fix Supplementary Table names.
</commit_message>
<xml_diff>
--- a/supplementary_tables/Supplementary_Tables.xlsx
+++ b/supplementary_tables/Supplementary_Tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ianhoskins/satmut_utils_supplementary/supplementary_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13340F8D-4E7F-1C40-8864-264F71B1DD17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89E9270A-8AB4-E745-B926-AAB894FB781A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="780" windowWidth="31440" windowHeight="19340" activeTab="3" xr2:uid="{1B22F140-15A2-E942-BFF5-E35174637834}"/>
+    <workbookView xWindow="2620" yWindow="780" windowWidth="31440" windowHeight="19340" xr2:uid="{1B22F140-15A2-E942-BFF5-E35174637834}"/>
   </bookViews>
   <sheets>
     <sheet name="Supplementary_Table_1" sheetId="1" r:id="rId1"/>
@@ -1704,16 +1704,16 @@
     <t>CBS_deficiency_position</t>
   </si>
   <si>
-    <t>Supplementary Table 3: CBS tail-less primers for RACE-like, Anchored Multiplex PCR chemistry</t>
-  </si>
-  <si>
-    <t>Supplementary Table 2: pDEST_HC_Rec_Bxb_v2_CBS PCR1 and PCR2 primers for amplicon chemistry</t>
-  </si>
-  <si>
-    <t>Supplementary Table 1: Variants with differntial RNA abundance by amplicon and RACE-like chemistries</t>
-  </si>
-  <si>
     <t>Supplementary Table 4: CBS primers for negative control library amplification</t>
+  </si>
+  <si>
+    <t>Supplementary Table 1: Variants with differential RNA abundance by amplicon and RACE-like methods</t>
+  </si>
+  <si>
+    <t>Supplementary Table 2: pDEST_HC_Rec_Bxb_v2_CBS PCR1 and PCR2 primers for amplicon method</t>
+  </si>
+  <si>
+    <t>Supplementary Table 3: CBS tail-less primers for RACE-like, Anchored Multiplex PCR method</t>
   </si>
 </sst>
 </file>
@@ -2131,7 +2131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CDD16E8-C7C2-B243-8EF3-648BE6A0AF40}">
   <dimension ref="A1:T113"/>
   <sheetViews>
-    <sheetView zoomScale="68" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2149,7 +2149,7 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
@@ -9241,9 +9241,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8FDA9B2-4331-D645-B520-C73E316232B4}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9253,7 +9251,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -9331,7 +9329,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -9864,7 +9862,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17773C0-4ECC-EB44-AC66-28028E35A7C1}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -9876,7 +9874,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
IH 29MAR2023 updated Additional file 1 and Supplementary Tables, added Additional file 2.
</commit_message>
<xml_diff>
--- a/supplementary_tables/Supplementary_Tables.xlsx
+++ b/supplementary_tables/Supplementary_Tables.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ianhoskins/satmut_utils_supplementary/supplementary_tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B83F2B-1FC9-C043-BB56-B52B8B18C759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5F41F37-FAF1-D242-9800-CF4C55696B21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2620" yWindow="760" windowWidth="31440" windowHeight="19340" xr2:uid="{1B22F140-15A2-E942-BFF5-E35174637834}"/>
+    <workbookView xWindow="2620" yWindow="740" windowWidth="31440" windowHeight="19340" xr2:uid="{1B22F140-15A2-E942-BFF5-E35174637834}"/>
   </bookViews>
   <sheets>
-    <sheet name="Supplementary_Table_1" sheetId="5" r:id="rId1"/>
-    <sheet name="Supplementary_Table_2" sheetId="1" r:id="rId2"/>
-    <sheet name="Supplementary_Table_3" sheetId="4" r:id="rId3"/>
-    <sheet name="Supplementary_Table_4" sheetId="3" r:id="rId4"/>
-    <sheet name="Supplementary_Table_5" sheetId="2" r:id="rId5"/>
+    <sheet name="Table_S1" sheetId="5" r:id="rId1"/>
+    <sheet name="Table_S2" sheetId="1" r:id="rId2"/>
+    <sheet name="Table_S3" sheetId="4" r:id="rId3"/>
+    <sheet name="Table_S4" sheetId="3" r:id="rId4"/>
+    <sheet name="Table_S5" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2944,19 +2944,19 @@
     <t>DOWN_REF_NT:T</t>
   </si>
   <si>
-    <t>Supplementary Table 5: CBS primers for negative control library amplification</t>
-  </si>
-  <si>
-    <t>Supplementary Table 4: CBS tail-less primers for RACE-like, Anchored Multiplex PCR method</t>
-  </si>
-  <si>
-    <t>Supplementary Table 3: pDEST_HC_Rec_Bxb_v2_CBS PCR1 and PCR2 primers for amplicon method</t>
-  </si>
-  <si>
-    <t>Supplementary Table 1: satmut_utils 'call' error correction features</t>
-  </si>
-  <si>
-    <t>Supplementary Table 2: Variants with differential RNA abundance by amplicon and RACE-like methods</t>
+    <t>Table S1: satmut_utils 'call' error correction features</t>
+  </si>
+  <si>
+    <t>Table S2: Variants with differential RNA abundance by amplicon and RACE-like methods</t>
+  </si>
+  <si>
+    <t>Table S3: pDEST_HC_Rec_Bxb_v2_CBS PCR1 and PCR2 primers for amplicon method</t>
+  </si>
+  <si>
+    <t>Table S4: CBS tail-less primers for RACE-like, Anchored Multiplex PCR method</t>
+  </si>
+  <si>
+    <t>Table S5: CBS primers for negative control library amplification</t>
   </si>
 </sst>
 </file>
@@ -3011,7 +3011,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3019,9 +3019,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3396,7 +3393,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>941</v>
+        <v>938</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -3633,11 +3630,15 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="4"/>
-    <col min="2" max="2" width="41.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="10.83203125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="50.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="6" width="10.83203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="4" customWidth="1"/>
     <col min="10" max="10" width="15" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.83203125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="19.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" style="4" customWidth="1"/>
     <col min="14" max="14" width="14" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="19.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.1640625" style="4" customWidth="1"/>
@@ -3645,13 +3646,14 @@
     <col min="19" max="19" width="8.5" style="4" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="21.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="21" max="25" width="10.83203125" style="4"/>
-    <col min="26" max="26" width="17.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="10.83203125" style="4"/>
+    <col min="26" max="26" width="21.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>942</v>
+        <v>939</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
@@ -3737,7 +3739,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="3" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -3821,7 +3823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>0</v>
       </c>
@@ -3900,9 +3902,8 @@
       <c r="Z4" s="4" t="s">
         <v>492</v>
       </c>
-      <c r="AA4" s="4"/>
-    </row>
-    <row r="5" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
@@ -3986,7 +3987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -4070,7 +4071,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>0</v>
       </c>
@@ -4149,9 +4150,8 @@
       <c r="Z7" s="4" t="s">
         <v>495</v>
       </c>
-      <c r="AA7" s="4"/>
-    </row>
-    <row r="8" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>0</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
@@ -4319,7 +4319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>0</v>
       </c>
@@ -4403,7 +4403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>0</v>
       </c>
@@ -4487,7 +4487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>0</v>
       </c>
@@ -4571,7 +4571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>0</v>
       </c>
@@ -4655,7 +4655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>0</v>
       </c>
@@ -4734,9 +4734,8 @@
       <c r="Z14" s="4" t="s">
         <v>502</v>
       </c>
-      <c r="AA14" s="4"/>
-    </row>
-    <row r="15" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>0</v>
       </c>
@@ -4820,7 +4819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>0</v>
       </c>
@@ -4904,7 +4903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>0</v>
       </c>
@@ -4983,9 +4982,8 @@
       <c r="Z17" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="AA17" s="4"/>
-    </row>
-    <row r="18" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>0</v>
       </c>
@@ -5069,7 +5067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>0</v>
       </c>
@@ -5153,7 +5151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>0</v>
       </c>
@@ -5237,7 +5235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>0</v>
       </c>
@@ -5321,7 +5319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>0</v>
       </c>
@@ -5405,7 +5403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>0</v>
       </c>
@@ -5489,7 +5487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>0</v>
       </c>
@@ -5573,7 +5571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>0</v>
       </c>
@@ -5657,7 +5655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>0</v>
       </c>
@@ -5741,7 +5739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>0</v>
       </c>
@@ -5825,7 +5823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>0</v>
       </c>
@@ -5909,7 +5907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>0</v>
       </c>
@@ -5993,7 +5991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>0</v>
       </c>
@@ -6077,7 +6075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>0</v>
       </c>
@@ -6161,7 +6159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>0</v>
       </c>
@@ -6245,7 +6243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>0</v>
       </c>
@@ -6329,7 +6327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>0</v>
       </c>
@@ -6413,7 +6411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>0</v>
       </c>
@@ -6492,9 +6490,8 @@
       <c r="Z35" s="4" t="s">
         <v>533</v>
       </c>
-      <c r="AA35" s="4"/>
-    </row>
-    <row r="36" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>0</v>
       </c>
@@ -6578,7 +6575,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>0</v>
       </c>
@@ -6662,7 +6659,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>0</v>
       </c>
@@ -6746,7 +6743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>0</v>
       </c>
@@ -6830,7 +6827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>0</v>
       </c>
@@ -6914,7 +6911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>0</v>
       </c>
@@ -6998,7 +6995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>0</v>
       </c>
@@ -7082,7 +7079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>0</v>
       </c>
@@ -7166,7 +7163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>0</v>
       </c>
@@ -7250,7 +7247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>0</v>
       </c>
@@ -7334,7 +7331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>0</v>
       </c>
@@ -7418,7 +7415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>0</v>
       </c>
@@ -7502,7 +7499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>0</v>
       </c>
@@ -7586,7 +7583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>0</v>
       </c>
@@ -7670,7 +7667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>0</v>
       </c>
@@ -7754,7 +7751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>0</v>
       </c>
@@ -7838,7 +7835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>0</v>
       </c>
@@ -7922,7 +7919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>0</v>
       </c>
@@ -8006,7 +8003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>0</v>
       </c>
@@ -8090,7 +8087,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>0</v>
       </c>
@@ -8174,7 +8171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>0</v>
       </c>
@@ -8258,7 +8255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>0</v>
       </c>
@@ -8342,7 +8339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>0</v>
       </c>
@@ -8426,7 +8423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>0</v>
       </c>
@@ -8499,7 +8496,7 @@
       <c r="X59" s="4">
         <v>0.67183945017574898</v>
       </c>
-      <c r="Y59" s="6">
+      <c r="Y59" s="5">
         <v>5.8352999999997102E-5</v>
       </c>
       <c r="Z59" s="4" t="s">
@@ -8510,7 +8507,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>0</v>
       </c>
@@ -8594,7 +8591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>0</v>
       </c>
@@ -8678,7 +8675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>0</v>
       </c>
@@ -8762,7 +8759,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>0</v>
       </c>
@@ -8846,7 +8843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>0</v>
       </c>
@@ -8930,7 +8927,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>0</v>
       </c>
@@ -9014,7 +9011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>0</v>
       </c>
@@ -9098,7 +9095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>0</v>
       </c>
@@ -9182,7 +9179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>0</v>
       </c>
@@ -9266,7 +9263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>0</v>
       </c>
@@ -9350,7 +9347,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>0</v>
       </c>
@@ -9434,7 +9431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>0</v>
       </c>
@@ -9518,7 +9515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>0</v>
       </c>
@@ -9602,7 +9599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>0</v>
       </c>
@@ -9686,7 +9683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>0</v>
       </c>
@@ -9770,7 +9767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>0</v>
       </c>
@@ -9854,7 +9851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>0</v>
       </c>
@@ -9938,7 +9935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>0</v>
       </c>
@@ -10022,7 +10019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>182</v>
       </c>
@@ -10106,7 +10103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>182</v>
       </c>
@@ -10185,9 +10182,8 @@
       <c r="Z79" s="4" t="s">
         <v>597</v>
       </c>
-      <c r="AA79" s="4"/>
-    </row>
-    <row r="80" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="80" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>182</v>
       </c>
@@ -10271,7 +10267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>182</v>
       </c>
@@ -10355,7 +10351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>182</v>
       </c>
@@ -10434,9 +10430,8 @@
       <c r="Z82" s="4" t="s">
         <v>604</v>
       </c>
-      <c r="AA82" s="4"/>
-    </row>
-    <row r="83" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>182</v>
       </c>
@@ -10520,7 +10515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>182</v>
       </c>
@@ -10604,7 +10599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>182</v>
       </c>
@@ -10688,7 +10683,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>182</v>
       </c>
@@ -10772,7 +10767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>182</v>
       </c>
@@ -10856,7 +10851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>182</v>
       </c>
@@ -10940,7 +10935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
         <v>182</v>
       </c>
@@ -11024,7 +11019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>182</v>
       </c>
@@ -11108,7 +11103,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
         <v>182</v>
       </c>
@@ -11192,7 +11187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>182</v>
       </c>
@@ -11276,7 +11271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>182</v>
       </c>
@@ -11360,7 +11355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>182</v>
       </c>
@@ -11444,7 +11439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>182</v>
       </c>
@@ -11528,7 +11523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>182</v>
       </c>
@@ -11612,7 +11607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>182</v>
       </c>
@@ -11696,7 +11691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>182</v>
       </c>
@@ -11780,7 +11775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>182</v>
       </c>
@@ -11864,7 +11859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
         <v>182</v>
       </c>
@@ -11943,9 +11938,8 @@
       <c r="Z100" s="4" t="s">
         <v>633</v>
       </c>
-      <c r="AA100" s="4"/>
-    </row>
-    <row r="101" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="101" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
         <v>182</v>
       </c>
@@ -12029,7 +12023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
         <v>182</v>
       </c>
@@ -12113,7 +12107,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
         <v>182</v>
       </c>
@@ -12197,7 +12191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>182</v>
       </c>
@@ -12281,7 +12275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>182</v>
       </c>
@@ -12365,7 +12359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>182</v>
       </c>
@@ -12449,7 +12443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:27" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>182</v>
       </c>
@@ -20759,7 +20753,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8FDA9B2-4331-D645-B520-C73E316232B4}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20769,7 +20765,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>940</v>
       </c>
     </row>
@@ -20838,7 +20834,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D578B66-DD34-FD41-AAAD-5C3CC01DF027}">
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20848,8 +20846,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>939</v>
+      <c r="A1" s="6" t="s">
+        <v>941</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -21382,18 +21380,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E17773C0-4ECC-EB44-AC66-28028E35A7C1}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="183.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="56.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>938</v>
+      <c r="A1" s="6" t="s">
+        <v>942</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>